<commit_message>
Replace backend structure with new one
</commit_message>
<xml_diff>
--- a/backend/data/DIT333 Fake Course.xlsx
+++ b/backend/data/DIT333 Fake Course.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gomesf/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intisar Abdi\Downloads\panda_exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C966148-9DB6-A94F-9853-DCC39EE2FBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359C71E5-3A97-4818-AB53-A57B7D8947D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VariableView" sheetId="1" r:id="rId1"/>
@@ -33,30 +33,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="101">
   <si>
     <t>Variable Name</t>
   </si>
@@ -296,9 +274,6 @@
     <t>1. Physical computing aspect  2. Weekly reflection tasks  3. Open Q&amp;A style lectures</t>
   </si>
   <si>
-    <t>What are the three things you liked the least about the course?</t>
-  </si>
-  <si>
     <t>Sometimes the lectures felt too long, especially in the afternoon sessions.</t>
   </si>
   <si>
@@ -308,9 +283,6 @@
     <t>1. Lack of full lecture recordings  2. Too much theory before hands-on parts  3. Unclear deadlines</t>
   </si>
   <si>
-    <t>Too many overlapping deadlines with other courses.</t>
-  </si>
-  <si>
     <t>The feedback on assignments took too long.</t>
   </si>
   <si>
@@ -332,9 +304,6 @@
     <t>Sometimes the teacher spoke too fast for me to follow.</t>
   </si>
   <si>
-    <t>The course assumed too much prior knowledge at the start.</t>
-  </si>
-  <si>
     <t>The field trip was cool but took a lot of time during a busy week.</t>
   </si>
   <si>
@@ -345,9 +314,6 @@
   </si>
   <si>
     <t>Nothing major, but some lectures could be more engaging.</t>
-  </si>
-  <si>
-    <t>There was too much time spent on repetitive examples.</t>
   </si>
   <si>
     <t>TA availability was limited in the weeks before the deadline.</t>
@@ -754,19 +720,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="150.1640625" customWidth="1"/>
-    <col min="3" max="3" width="27.1640625" customWidth="1"/>
+    <col min="2" max="2" width="150.109375" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -786,7 +752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -806,7 +772,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -826,7 +792,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -846,7 +812,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -866,7 +832,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -886,7 +852,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -906,7 +872,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -926,7 +892,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -946,7 +912,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -966,7 +932,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -986,7 +952,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1006,7 +972,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1026,7 +992,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1046,7 +1012,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1066,7 +1032,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1086,7 +1052,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -1106,7 +1072,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1133,20 +1099,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R76"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16" width="9.1640625" customWidth="1"/>
+    <col min="1" max="16" width="9.109375" customWidth="1"/>
     <col min="17" max="17" width="132.6640625" customWidth="1"/>
     <col min="18" max="18" width="1425.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1202,7 +1168,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1255,10 +1221,10 @@
         <v>50</v>
       </c>
       <c r="R2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1311,10 +1277,10 @@
         <v>51</v>
       </c>
       <c r="R3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1367,10 +1333,10 @@
         <v>67</v>
       </c>
       <c r="R4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1423,7 +1389,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
@@ -1473,10 +1439,10 @@
         <v>5</v>
       </c>
       <c r="R6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1529,10 +1495,10 @@
         <v>68</v>
       </c>
       <c r="R7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -1585,10 +1551,10 @@
         <v>53</v>
       </c>
       <c r="R8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -1641,10 +1607,10 @@
         <v>54</v>
       </c>
       <c r="R9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0</v>
       </c>
@@ -1697,10 +1663,10 @@
         <v>55</v>
       </c>
       <c r="R10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0</v>
       </c>
@@ -1753,10 +1719,10 @@
         <v>69</v>
       </c>
       <c r="R11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0</v>
       </c>
@@ -1809,10 +1775,10 @@
         <v>56</v>
       </c>
       <c r="R12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0</v>
       </c>
@@ -1865,7 +1831,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
@@ -1915,7 +1881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>
@@ -1968,10 +1934,10 @@
         <v>72</v>
       </c>
       <c r="R15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0</v>
       </c>
@@ -2024,10 +1990,10 @@
         <v>57</v>
       </c>
       <c r="R16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0</v>
       </c>
@@ -2080,10 +2046,10 @@
         <v>58</v>
       </c>
       <c r="R17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
@@ -2136,10 +2102,10 @@
         <v>71</v>
       </c>
       <c r="R18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
@@ -2192,7 +2158,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0</v>
       </c>
@@ -2245,10 +2211,10 @@
         <v>60</v>
       </c>
       <c r="R20" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -2280,7 +2246,7 @@
         <v>3</v>
       </c>
       <c r="K21">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="L21">
         <v>2</v>
@@ -2298,10 +2264,10 @@
         <v>5</v>
       </c>
       <c r="R21" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0</v>
       </c>
@@ -2354,10 +2320,10 @@
         <v>73</v>
       </c>
       <c r="R22" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0</v>
       </c>
@@ -2410,10 +2376,10 @@
         <v>61</v>
       </c>
       <c r="R23" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>0</v>
       </c>
@@ -2466,10 +2432,10 @@
         <v>62</v>
       </c>
       <c r="R24" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>0</v>
       </c>
@@ -2522,10 +2488,10 @@
         <v>74</v>
       </c>
       <c r="R25" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0</v>
       </c>
@@ -2578,10 +2544,10 @@
         <v>63</v>
       </c>
       <c r="R26" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0</v>
       </c>
@@ -2634,10 +2600,10 @@
         <v>64</v>
       </c>
       <c r="R27" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>0</v>
       </c>
@@ -2690,10 +2656,10 @@
         <v>65</v>
       </c>
       <c r="R28" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>0</v>
       </c>
@@ -2746,173 +2712,17 @@
         <v>66</v>
       </c>
       <c r="R29" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="R30" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="R31" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="46" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J46" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="47" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J47" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="48" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J48" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="49" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J49" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="50" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J50" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="51" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J51" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="52" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J52" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="53" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J53" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="54" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J54" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="55" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J55" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="56" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J56" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="57" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J57" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="58" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J58" t="e" cm="1">
-        <f t="array" ref="J58">- Confusing lab instructions  - Hard to get help during lab sessions  - Sparse grading rubric</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="59" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J59" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="60" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J60" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="61" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J61" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="62" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J62" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="63" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J63" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="64" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J64" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="65" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J65" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="66" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J66" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="67" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J67" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="68" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J68" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="69" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J69" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="70" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J70" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="71" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J71" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="72" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J72" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="73" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J73" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="74" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J74" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="75" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J75" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="76" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J76" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2921,26 +2731,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="209be723-9c8f-46e9-af51-e534829a174b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="6815e5c0-48ab-4933-89c2-49f87de7d26d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100202D199910A9094DB83C608A83057450" ma:contentTypeVersion="17" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="94577e9aac6e2f61595bbc6564328673">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="209be723-9c8f-46e9-af51-e534829a174b" xmlns:ns3="6815e5c0-48ab-4933-89c2-49f87de7d26d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ab2ccaf7dd11a5d4a16f5855c8d69ffd" ns2:_="" ns3:_="">
     <xsd:import namespace="209be723-9c8f-46e9-af51-e534829a174b"/>
@@ -3187,26 +2977,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F57E168-3102-4B6F-9070-10F264801D2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="209be723-9c8f-46e9-af51-e534829a174b"/>
-    <ds:schemaRef ds:uri="6815e5c0-48ab-4933-89c2-49f87de7d26d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BA0BC3B-CFE3-41A7-AB0D-201D3AEC745B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="209be723-9c8f-46e9-af51-e534829a174b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="6815e5c0-48ab-4933-89c2-49f87de7d26d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9CDC52D-66B4-4CFE-BBBF-AD0C2E54CE47}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3223,4 +3014,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BA0BC3B-CFE3-41A7-AB0D-201D3AEC745B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F57E168-3102-4B6F-9070-10F264801D2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="209be723-9c8f-46e9-af51-e534829a174b"/>
+    <ds:schemaRef ds:uri="6815e5c0-48ab-4933-89c2-49f87de7d26d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
#11 Create json file with questions and answers from course evaluation
</commit_message>
<xml_diff>
--- a/backend/data/DIT333 Fake Course.xlsx
+++ b/backend/data/DIT333 Fake Course.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gomesf/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renaa\.vscode\starling-vox\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C966148-9DB6-A94F-9853-DCC39EE2FBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{66CF63B4-41D2-474A-8487-79103B6C4CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VariableView" sheetId="1" r:id="rId1"/>
@@ -33,30 +33,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="97">
   <si>
     <t>Variable Name</t>
   </si>
@@ -71,9 +49,6 @@
   </si>
   <si>
     <t>Value Codes</t>
-  </si>
-  <si>
-    <t>Missing Code</t>
   </si>
   <si>
     <t>VAR00</t>
@@ -209,9 +184,6 @@
     <t>none</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>VAR16</t>
   </si>
   <si>
@@ -296,9 +268,6 @@
     <t>1. Physical computing aspect  2. Weekly reflection tasks  3. Open Q&amp;A style lectures</t>
   </si>
   <si>
-    <t>What are the three things you liked the least about the course?</t>
-  </si>
-  <si>
     <t>Sometimes the lectures felt too long, especially in the afternoon sessions.</t>
   </si>
   <si>
@@ -308,9 +277,6 @@
     <t>1. Lack of full lecture recordings  2. Too much theory before hands-on parts  3. Unclear deadlines</t>
   </si>
   <si>
-    <t>Too many overlapping deadlines with other courses.</t>
-  </si>
-  <si>
     <t>The feedback on assignments took too long.</t>
   </si>
   <si>
@@ -332,9 +298,6 @@
     <t>Sometimes the teacher spoke too fast for me to follow.</t>
   </si>
   <si>
-    <t>The course assumed too much prior knowledge at the start.</t>
-  </si>
-  <si>
     <t>The field trip was cool but took a lot of time during a busy week.</t>
   </si>
   <si>
@@ -347,9 +310,6 @@
     <t>Nothing major, but some lectures could be more engaging.</t>
   </si>
   <si>
-    <t>There was too much time spent on repetitive examples.</t>
-  </si>
-  <si>
     <t>TA availability was limited in the weeks before the deadline.</t>
   </si>
   <si>
@@ -378,12 +338,6 @@
   </si>
   <si>
     <t>Lecture times changed a lot, which was confusing.</t>
-  </si>
-  <si>
-    <t>The bonus tasks were too hard and not explained well.</t>
-  </si>
-  <si>
-    <t>1. Disorganized lab sessions  2. Lack of answers for quizzes  3. Not enough diversity in topics</t>
   </si>
 </sst>
 </file>
@@ -752,21 +706,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="150.1640625" customWidth="1"/>
-    <col min="3" max="3" width="27.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.36328125" customWidth="1"/>
+    <col min="2" max="2" width="150.1796875" customWidth="1"/>
+    <col min="3" max="3" width="27.1796875" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -782,427 +738,374 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="F2">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E5" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E6" t="s">
         <v>9</v>
       </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E8" t="s">
         <v>9</v>
       </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>24</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E10" t="s">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="C11" t="s">
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
         <v>8</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E12" t="s">
         <v>9</v>
       </c>
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
         <v>8</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E13" t="s">
         <v>9</v>
       </c>
-      <c r="E12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
         <v>8</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E14" t="s">
         <v>9</v>
       </c>
-      <c r="E13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>34</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
         <v>8</v>
       </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="E15" t="s">
         <v>36</v>
       </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
         <v>8</v>
       </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="E16" t="s">
         <v>39</v>
       </c>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>40</v>
       </c>
-      <c r="F16">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>41</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>42</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>43</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>44</v>
       </c>
-      <c r="E17" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>45</v>
       </c>
-      <c r="F17" t="s">
+      <c r="B18" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" t="s">
-        <v>48</v>
-      </c>
       <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
         <v>43</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>44</v>
-      </c>
-      <c r="E18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R76"/>
+  <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView topLeftCell="A9" zoomScale="46" workbookViewId="0">
+      <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16" width="9.1640625" customWidth="1"/>
-    <col min="17" max="17" width="132.6640625" customWidth="1"/>
-    <col min="18" max="18" width="1425.33203125" customWidth="1"/>
+    <col min="1" max="16" width="9.1796875" customWidth="1"/>
+    <col min="17" max="17" width="132.6328125" customWidth="1"/>
+    <col min="18" max="18" width="1425.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1252,13 +1155,13 @@
         <v>3</v>
       </c>
       <c r="Q2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1308,13 +1211,13 @@
         <v>3</v>
       </c>
       <c r="Q3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="R3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1364,13 +1267,13 @@
         <v>4</v>
       </c>
       <c r="Q4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1420,10 +1323,10 @@
         <v>4</v>
       </c>
       <c r="Q5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0</v>
       </c>
@@ -1473,10 +1376,10 @@
         <v>5</v>
       </c>
       <c r="R6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1526,13 +1429,13 @@
         <v>3</v>
       </c>
       <c r="Q7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="R7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0</v>
       </c>
@@ -1582,13 +1485,13 @@
         <v>4</v>
       </c>
       <c r="Q8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="R8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0</v>
       </c>
@@ -1638,13 +1541,13 @@
         <v>4</v>
       </c>
       <c r="Q9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="R9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0</v>
       </c>
@@ -1694,13 +1597,13 @@
         <v>4</v>
       </c>
       <c r="Q10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0</v>
       </c>
@@ -1750,13 +1653,13 @@
         <v>4</v>
       </c>
       <c r="Q11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0</v>
       </c>
@@ -1806,13 +1709,13 @@
         <v>4</v>
       </c>
       <c r="Q12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="R12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0</v>
       </c>
@@ -1862,10 +1765,10 @@
         <v>4</v>
       </c>
       <c r="Q13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0</v>
       </c>
@@ -1915,7 +1818,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0</v>
       </c>
@@ -1965,13 +1868,13 @@
         <v>4</v>
       </c>
       <c r="Q15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="R15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0</v>
       </c>
@@ -2021,13 +1924,13 @@
         <v>3</v>
       </c>
       <c r="Q16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="R16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>0</v>
       </c>
@@ -2077,13 +1980,13 @@
         <v>1</v>
       </c>
       <c r="Q17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="R17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0</v>
       </c>
@@ -2133,13 +2036,13 @@
         <v>3</v>
       </c>
       <c r="Q18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="R18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>0</v>
       </c>
@@ -2189,10 +2092,10 @@
         <v>5</v>
       </c>
       <c r="Q19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>0</v>
       </c>
@@ -2242,13 +2145,13 @@
         <v>5</v>
       </c>
       <c r="Q20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R20" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>0</v>
       </c>
@@ -2280,7 +2183,7 @@
         <v>3</v>
       </c>
       <c r="K21">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="L21">
         <v>2</v>
@@ -2298,10 +2201,10 @@
         <v>5</v>
       </c>
       <c r="R21" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>0</v>
       </c>
@@ -2351,13 +2254,13 @@
         <v>2</v>
       </c>
       <c r="Q22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="R22" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>0</v>
       </c>
@@ -2407,13 +2310,13 @@
         <v>5</v>
       </c>
       <c r="Q23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R23" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>0</v>
       </c>
@@ -2463,13 +2366,13 @@
         <v>3</v>
       </c>
       <c r="Q24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R24" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>0</v>
       </c>
@@ -2519,13 +2422,13 @@
         <v>1</v>
       </c>
       <c r="Q25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="R25" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>0</v>
       </c>
@@ -2575,13 +2478,13 @@
         <v>5</v>
       </c>
       <c r="Q26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R26" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>0</v>
       </c>
@@ -2631,13 +2534,13 @@
         <v>5</v>
       </c>
       <c r="Q27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R27" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>0</v>
       </c>
@@ -2687,13 +2590,13 @@
         <v>5</v>
       </c>
       <c r="Q28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R28" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>0</v>
       </c>
@@ -2743,204 +2646,19 @@
         <v>5</v>
       </c>
       <c r="Q29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R29" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R30" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R31" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="46" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J46" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="47" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J47" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="48" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J48" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="49" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J49" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="50" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J50" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="51" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J51" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="52" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J52" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="53" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J53" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="54" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J54" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="55" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J55" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="56" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J56" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="57" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J57" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="58" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J58" t="e" cm="1">
-        <f t="array" ref="J58">- Confusing lab instructions  - Hard to get help during lab sessions  - Sparse grading rubric</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="59" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J59" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="60" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J60" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="61" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J61" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="62" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J62" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="63" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J63" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="64" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J64" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="65" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J65" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="66" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J66" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="67" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J67" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="68" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J68" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="69" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J69" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="70" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J70" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="71" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J71" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="72" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J72" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="73" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J73" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="74" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J74" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="75" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J75" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="76" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J76" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="209be723-9c8f-46e9-af51-e534829a174b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="6815e5c0-48ab-4933-89c2-49f87de7d26d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100202D199910A9094DB83C608A83057450" ma:contentTypeVersion="17" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="94577e9aac6e2f61595bbc6564328673">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="209be723-9c8f-46e9-af51-e534829a174b" xmlns:ns3="6815e5c0-48ab-4933-89c2-49f87de7d26d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ab2ccaf7dd11a5d4a16f5855c8d69ffd" ns2:_="" ns3:_="">
     <xsd:import namespace="209be723-9c8f-46e9-af51-e534829a174b"/>
@@ -3187,26 +2905,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F57E168-3102-4B6F-9070-10F264801D2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="209be723-9c8f-46e9-af51-e534829a174b"/>
-    <ds:schemaRef ds:uri="6815e5c0-48ab-4933-89c2-49f87de7d26d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BA0BC3B-CFE3-41A7-AB0D-201D3AEC745B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="209be723-9c8f-46e9-af51-e534829a174b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="6815e5c0-48ab-4933-89c2-49f87de7d26d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9CDC52D-66B4-4CFE-BBBF-AD0C2E54CE47}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3223,4 +2942,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BA0BC3B-CFE3-41A7-AB0D-201D3AEC745B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F57E168-3102-4B6F-9070-10F264801D2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="209be723-9c8f-46e9-af51-e534829a174b"/>
+    <ds:schemaRef ds:uri="6815e5c0-48ab-4933-89c2-49f87de7d26d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>